<commit_message>
Sterility Counts, Strat by indication for obj3,4, counts per ATCs
</commit_message>
<xml_diff>
--- a/RAM_scripts/p_steps/codelists/ATC_lot4_formatted.xlsx
+++ b/RAM_scripts/p_steps/codelists/ATC_lot4_formatted.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgamb\Documents\GitHub\RAM_STUDY\RAM_scripts\p_steps\codelists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1BD2C6-6FC7-449A-A2C5-1F2EABD2D62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA0124A-0550-407F-87C2-8059164BC690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="203">
   <si>
     <t>Benzoyl peroxide (local)</t>
   </si>
@@ -620,13 +620,25 @@
   </si>
   <si>
     <t>S01AA17</t>
+  </si>
+  <si>
+    <t>A11CA01</t>
+  </si>
+  <si>
+    <t>Oral A vitamin</t>
+  </si>
+  <si>
+    <t>Tetracycline</t>
+  </si>
+  <si>
+    <t>J01AA07</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -782,6 +794,19 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1126,7 +1151,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1134,6 +1159,8 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2378,10 +2405,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B32"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2414,41 +2441,41 @@
         <v>137</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>24</v>
+        <v>200</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>24</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>137</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>29</v>
+      <c r="B3" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>18</v>
+      <c r="B4" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -2456,13 +2483,13 @@
         <v>137</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -2470,13 +2497,13 @@
         <v>137</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -2484,13 +2511,13 @@
         <v>137</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -2498,13 +2525,13 @@
         <v>137</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -2512,41 +2539,41 @@
         <v>137</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>137</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>137</v>
-      </c>
-      <c r="B10" s="4" t="s">
+    <row r="11" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>144</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>137</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -2554,13 +2581,13 @@
         <v>137</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>182</v>
+        <v>5</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -2568,13 +2595,13 @@
         <v>137</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -2582,13 +2609,13 @@
         <v>137</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -2596,13 +2623,13 @@
         <v>137</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -2610,13 +2637,13 @@
         <v>137</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -2624,13 +2651,13 @@
         <v>137</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -2638,13 +2665,13 @@
         <v>137</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -2652,13 +2679,13 @@
         <v>137</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -2666,13 +2693,13 @@
         <v>137</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -2680,13 +2707,13 @@
         <v>137</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -2694,13 +2721,13 @@
         <v>137</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -2708,13 +2735,13 @@
         <v>137</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -2722,13 +2749,13 @@
         <v>137</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -2736,13 +2763,13 @@
         <v>137</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -2750,13 +2777,13 @@
         <v>137</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -2764,13 +2791,13 @@
         <v>137</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -2778,13 +2805,13 @@
         <v>137</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>17</v>
+        <v>197</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -2792,13 +2819,13 @@
         <v>137</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -2806,13 +2833,13 @@
         <v>137</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -2820,32 +2847,66 @@
         <v>137</v>
       </c>
       <c r="B31" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>137</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C32" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E32" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>137</v>
-      </c>
-      <c r="B32" s="4" t="s">
+    <row r="33" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>137</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C33" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E33" s="4" t="s">
         <v>14</v>
       </c>
     </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>137</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B36" s="5"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="6"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F32">
-    <sortCondition ref="B2:B32"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F33">
+    <sortCondition ref="B2:B33"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Per indication code completed
</commit_message>
<xml_diff>
--- a/RAM_scripts/p_steps/codelists/ATC_lot4_formatted.xlsx
+++ b/RAM_scripts/p_steps/codelists/ATC_lot4_formatted.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgamb\Documents\GitHub\RAM_STUDY\RAM_scripts\p_steps\codelists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA0124A-0550-407F-87C2-8059164BC690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7F59AE-0FB3-4CA5-BDC9-A9E9DDE08CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Retinoid" sheetId="3" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="189">
   <si>
     <t>Benzoyl peroxide (local)</t>
   </si>
@@ -160,79 +160,37 @@
     <t>clobetasone </t>
   </si>
   <si>
-    <t>D07AB01 </t>
-  </si>
-  <si>
     <t>hydrocortisone butyrate </t>
   </si>
   <si>
-    <t>D07AB02 </t>
-  </si>
-  <si>
     <t>flumetasone </t>
   </si>
   <si>
-    <t>D07AB03 </t>
-  </si>
-  <si>
     <t>fluocortin </t>
   </si>
   <si>
-    <t>D07AB04 </t>
-  </si>
-  <si>
     <t>fluperolone </t>
   </si>
   <si>
-    <t>D07AB05 </t>
-  </si>
-  <si>
     <t>fluorometholone </t>
   </si>
   <si>
-    <t>D07AB06 </t>
-  </si>
-  <si>
     <t>fluprednidene </t>
   </si>
   <si>
-    <t>D07AB07 </t>
-  </si>
-  <si>
     <t>desonide </t>
   </si>
   <si>
-    <t>D07AB08 </t>
-  </si>
-  <si>
-    <t>D07AB09 </t>
-  </si>
-  <si>
     <t>alclometasone </t>
   </si>
   <si>
-    <t>D07AB10 </t>
-  </si>
-  <si>
     <t>hydrocortisone buteprate </t>
   </si>
   <si>
-    <t>D07AB11 </t>
-  </si>
-  <si>
-    <t>D07AB19 </t>
-  </si>
-  <si>
     <t>clocortolone </t>
   </si>
   <si>
-    <t>D07AB21 </t>
-  </si>
-  <si>
     <t>combinations of corticosteroids </t>
-  </si>
-  <si>
-    <t>D07AB30 </t>
   </si>
   <si>
     <t>fluclorolone </t>
@@ -1527,64 +1485,64 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1607,86 +1565,86 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>44</v>
@@ -1697,108 +1655,108 @@
     </row>
     <row r="7" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>151</v>
-      </c>
       <c r="C12" s="4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>36</v>
@@ -1809,38 +1767,38 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>29</v>
@@ -1851,38 +1809,38 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>28</v>
@@ -1893,52 +1851,52 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>30</v>
@@ -1949,450 +1907,450 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2407,8 +2365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2418,44 +2376,44 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>24</v>
@@ -2466,10 +2424,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>29</v>
@@ -2480,7 +2438,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>19</v>
@@ -2494,7 +2452,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>21</v>
@@ -2508,7 +2466,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>23</v>
@@ -2522,7 +2480,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>1</v>
@@ -2536,7 +2494,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>7</v>
@@ -2550,7 +2508,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>3</v>
@@ -2564,21 +2522,21 @@
     </row>
     <row r="11" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>5</v>
@@ -2592,10 +2550,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>25</v>
@@ -2606,10 +2564,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>26</v>
@@ -2620,10 +2578,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>27</v>
@@ -2634,10 +2592,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>28</v>
@@ -2648,10 +2606,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>29</v>
@@ -2662,10 +2620,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>30</v>
@@ -2676,10 +2634,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>24</v>
@@ -2690,10 +2648,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>31</v>
@@ -2704,10 +2662,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>36</v>
@@ -2718,10 +2676,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>37</v>
@@ -2732,10 +2690,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>38</v>
@@ -2746,10 +2704,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>39</v>
@@ -2760,10 +2718,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>40</v>
@@ -2774,10 +2732,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>41</v>
@@ -2788,10 +2746,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>42</v>
@@ -2802,10 +2760,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>43</v>
@@ -2816,7 +2774,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>17</v>
@@ -2830,7 +2788,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>10</v>
@@ -2844,7 +2802,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>13</v>
@@ -2858,10 +2816,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>11</v>
@@ -2872,7 +2830,7 @@
     </row>
     <row r="33" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>15</v>
@@ -2886,16 +2844,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -2916,8 +2874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2928,30 +2886,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>45</v>
+        <v>131</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>44</v>
@@ -2962,108 +2920,108 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>47</v>
+        <v>132</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>49</v>
+        <v>133</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>51</v>
+        <v>134</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>53</v>
+        <v>135</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>55</v>
+        <v>136</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="C8" s="4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>59</v>
+        <v>138</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>60</v>
+        <v>139</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>36</v>
@@ -3074,38 +3032,38 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>62</v>
+        <v>140</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>64</v>
+        <v>141</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>65</v>
+        <v>142</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>29</v>
@@ -3116,63 +3074,63 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>67</v>
+        <v>143</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>69</v>
+        <v>144</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>33</v>
@@ -3186,7 +3144,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>35</v>
@@ -3200,44 +3158,44 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>